<commit_message>
Polish the template for Netbook.
</commit_message>
<xml_diff>
--- a/netbook.xlsx
+++ b/netbook.xlsx
@@ -602,11 +602,11 @@
         <v>6</v>
       </c>
       <c r="H2" s="7" t="str">
-        <f aca="false">IF(EXACT(B11,"Discrete"), "B", "")</f>
+        <f aca="false">IF(EXACT(B11,"Discrete"), "B", "N/A")</f>
         <v>B</v>
       </c>
       <c r="I2" s="8" t="n">
-        <f aca="false">IF(AND(EXACT(B11,"Discrete"), B4&gt;=2, B6&gt;=2, EXACT(B12, "&gt;= 128-bit")), "C","")</f>
+        <f aca="false">IF(AND(EXACT(B11,"Discrete"), EXACT(B12, "&gt;= 128-bit"), B4&gt;=2, B6&gt;=2), "C", "N/A")</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reorder the output of Energy Star 5.2
</commit_message>
<xml_diff>
--- a/netbook.xlsx
+++ b/netbook.xlsx
@@ -113,7 +113,7 @@
     <t>GPU Frame Buffer Width</t>
   </si>
   <si>
-    <t>&gt;= 128-bit</t>
+    <t>&lt; 64-bit</t>
   </si>
   <si>
     <t>EP:</t>
@@ -553,7 +553,7 @@
   <dimension ref="A1:I65536"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I4" activeCellId="0" pane="topLeft" sqref="I4"/>
+      <selection activeCell="B11" activeCellId="0" pane="topLeft" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -602,11 +602,11 @@
         <v>6</v>
       </c>
       <c r="H2" s="7" t="str">
-        <f aca="false">IF(EXACT(B11,"Discrete"), "B", "N/A")</f>
+        <f aca="false">IF(EXACT(B11,"Discrete"), "B", "")</f>
         <v>B</v>
       </c>
       <c r="I2" s="8" t="n">
-        <f aca="false">IF(AND(EXACT(B11,"Discrete"), EXACT(B12, "&gt;= 128-bit"), B4&gt;=2, B6&gt;=2), "C", "N/A")</f>
+        <f aca="false">IF(AND(EXACT(B11,"Discrete"), EXACT(B12, "&gt;= 128-bit"), B4&gt;=2, B6&gt;=2), "C", "")</f>
         <v>0</v>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="H6" s="14" t="n">
         <f aca="false">IF(EXACT(H2,"B"), IF(EXACT(B12, "&lt; 64-bit"), 0, 3), "")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I6" s="14" t="str">
         <f aca="false">IF(EXACT(I2, "C"), 0, "")</f>
@@ -770,7 +770,7 @@
       </c>
       <c r="H8" s="19" t="n">
         <f aca="false">IF(EXACT(H2, "B"), H4+H5+H6+H7, "")</f>
-        <v>57.6</v>
+        <v>54.6</v>
       </c>
       <c r="I8" s="19" t="str">
         <f aca="false">IF(EXACT(I2, "C"), I4+I5+I6+I7, "")</f>
@@ -788,7 +788,7 @@
       </c>
       <c r="I9" s="20" t="str">
         <f aca="false">IF(EXACT(I2, "C"), IF(E8&lt;=I8, "PASS", "FAIL"), "")</f>
-        <v>PASS</v>
+        <v/>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="10">

</xml_diff>